<commit_message>
mise a jour 3
</commit_message>
<xml_diff>
--- a/data1/account.xlsx
+++ b/data1/account.xlsx
@@ -14272,7 +14272,7 @@
         <v>0</v>
       </c>
       <c r="N178">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="O178" t="inlineStr">
         <is>
@@ -33736,7 +33736,7 @@
         <v>2</v>
       </c>
       <c r="N427">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O427" t="inlineStr">
         <is>
@@ -51706,7 +51706,7 @@
         <v>0</v>
       </c>
       <c r="N657">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="O657" t="inlineStr">
         <is>

</xml_diff>